<commit_message>
Added book problem 3.70 Excel graph and values
</commit_message>
<xml_diff>
--- a/src/WrittenWorks/ExcelSheetWork/TailsProbabilities.xlsx
+++ b/src/WrittenWorks/ExcelSheetWork/TailsProbabilities.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a2fa70a607fc2c3/Documents/ProbandAppliedStats3327/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcti\IdeaProjects\ProbabilityandAppliedStatistics\src\WrittenWorks\ExcelSheetWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{3F3D360A-7342-4DD3-920D-B9213D8F9A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E29FA745-5EEC-4276-8C1B-975F8B9FFBAA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277D8783-B84E-4D2C-9843-F9432258B087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B658621B-17E1-48FF-9FD1-6E4C9BBF5D28}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B658621B-17E1-48FF-9FD1-6E4C9BBF5D28}"/>
   </bookViews>
   <sheets>
     <sheet name="Geo. Distribution Coin Graph" sheetId="1" r:id="rId1"/>
+    <sheet name="Book Problem 3.70" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>p (success)</t>
   </si>
@@ -83,9 +84,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +533,468 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Book Problem 3.70 (adding extra trials)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Book Problem 3.70'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>geo. distribution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Book Problem 3.70'!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.1920000000000048E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10240000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DF0B-4988-8A93-7597103799BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1048327216"/>
+        <c:axId val="1052514208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1048327216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Times</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1052514208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1052514208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Geometric</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Distribution Value</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1048327216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1076,6 +1537,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1097,6 +2061,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09119269-8EE1-2363-BD98-A254112E7F73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>307975</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68C4188A-6CFE-0251-2E60-1808CDE82372}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,8 +2441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A48F64-246C-42B5-B53F-18E344E94122}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1469,7 +2474,7 @@
         <f>((1-(1/2))^1)*(1/2)</f>
         <v>0.25</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2">
         <v>0.5</v>
       </c>
       <c r="M2">
@@ -1488,7 +2493,7 @@
         <f>((1-(1/2))^2)*(1/2)</f>
         <v>0.125</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3">
         <v>0.5</v>
       </c>
       <c r="M3">
@@ -1507,7 +2512,7 @@
         <f>((1-(1/2))^3)*(1/2)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4">
         <v>0.5</v>
       </c>
       <c r="M4">
@@ -1517,7 +2522,7 @@
         <v>3</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O3:O11" si="0">((L4)^(N4-1))*M4</f>
+        <f t="shared" ref="O4:O11" si="0">((L4)^(N4-1))*M4</f>
         <v>0.125</v>
       </c>
     </row>
@@ -1526,7 +2531,7 @@
         <f>((1-(1/2))^4)*(1/2)</f>
         <v>3.125E-2</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5">
         <v>0.5</v>
       </c>
       <c r="M5">
@@ -1545,7 +2550,7 @@
         <f>((1-(1/2))^5)*(1/2)</f>
         <v>1.5625E-2</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6">
         <v>0.5</v>
       </c>
       <c r="M6">
@@ -1564,7 +2569,7 @@
         <f>((1-(1/2))^6)*(1/2)</f>
         <v>7.8125E-3</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7">
         <v>0.5</v>
       </c>
       <c r="M7">
@@ -1583,7 +2588,7 @@
         <f>((1-(1/2))^7)*(1/2)</f>
         <v>3.90625E-3</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8">
         <v>0.5</v>
       </c>
       <c r="M8">
@@ -1602,7 +2607,7 @@
         <f>((1-(1/2))^8)*(1/2)</f>
         <v>1.953125E-3</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9">
         <v>0.5</v>
       </c>
       <c r="M9">
@@ -1621,7 +2626,7 @@
         <f>((1-(1/2))^9)*(1/2)</f>
         <v>9.765625E-4</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10">
         <v>0.5</v>
       </c>
       <c r="M10">
@@ -1636,7 +2641,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="L11" s="1">
+      <c r="L11">
         <v>0.5</v>
       </c>
       <c r="M11">
@@ -1648,6 +2653,115 @@
       <c r="O11">
         <f t="shared" si="0"/>
         <v>9.765625E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C479E424-A35E-4D99-836D-897E30F61000}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0.8</v>
+      </c>
+      <c r="B2">
+        <v>0.2</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <f>((A2)^(C2-1))*B2</f>
+        <v>8.1920000000000048E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0.8</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f>((A3)^(C3-1))*B3</f>
+        <v>0.10240000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0.8</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f>((A4)^(C4-1))*B4</f>
+        <v>0.12800000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0.8</v>
+      </c>
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>((A5)^(C5-1))*B5</f>
+        <v>0.16000000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0.8</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D3:D6" si="0">((A6)^(C6-1))*B6</f>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>